<commit_message>
FEAT: continuing cleanup of visibility fcns
see cleaning spreadsheet and main script changelog for details
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B4093D-36DA-4CC3-ADDF-7CF7CC8453EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F645448A-1D0A-49D8-B996-59CF0F16ADC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>Input checking?</t>
   </si>
   <si>
-    <t>Test/demo script exists?</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -193,13 +190,16 @@
   </si>
   <si>
     <t>Function compatible, test script not</t>
+  </si>
+  <si>
+    <t>Test script exists?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +217,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -352,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -377,6 +384,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,7 +704,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,13 +733,13 @@
         <v>49</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>44</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -792,7 +801,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="9"/>
       <c r="H6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,7 +815,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -820,7 +829,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1184,12 +1193,12 @@
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,24 +1219,24 @@
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1258,12 +1267,12 @@
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="10"/>
       <c r="H45" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FEAT: formatting and input checks for visibility
see main demo script changelog and cleaning spreadsheet for details
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F645448A-1D0A-49D8-B996-59CF0F16ADC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB3D35A-4C72-4A88-ACEB-708A0AB6C219}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Test script exists?</t>
+  </si>
+  <si>
+    <t>function deprecated</t>
+  </si>
+  <si>
+    <t>Combination 'test script' exists w/removeObstacle</t>
+  </si>
+  <si>
+    <t>Combination 'test script' exists w/addObstacle</t>
   </si>
 </sst>
 </file>
@@ -229,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,6 +281,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -359,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -386,6 +401,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,11 +720,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0B7FE0-246A-4335-9511-EB49E7B3228F}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +735,7 @@
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1064,12 +1084,12 @@
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,12 +1108,12 @@
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1181,12 +1201,12 @@
       <c r="A38" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="22"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1205,13 +1225,15 @@
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="2"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -1243,25 +1265,29 @@
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="2"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="2"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -1299,6 +1325,12 @@
         <v>47</v>
       </c>
     </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="21"/>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FEAT: added debug plotting for fcn_BoundedAStar_Astar
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB3D35A-4C72-4A88-ACEB-708A0AB6C219}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D998157-F620-4BB8-A8B2-A0BC02EA2A7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -723,8 +723,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +792,7 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="17"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>

</xml_diff>

<commit_message>
FEAT: working on updates to visibility test scripts
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D998157-F620-4BB8-A8B2-A0BC02EA2A7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABC2E22-B6A4-499A-B5D8-721EB4E511FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Scripts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -202,6 +203,15 @@
   </si>
   <si>
     <t>Combination 'test script' exists w/addObstacle</t>
+  </si>
+  <si>
+    <t>Are there test cases?</t>
+  </si>
+  <si>
+    <t>Uses fcn_MapGen_haltonVoronoiTiling</t>
+  </si>
+  <si>
+    <t>Plotting moved to fcn?</t>
   </si>
 </sst>
 </file>
@@ -238,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +294,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -406,6 +422,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,9 +742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0B7FE0-246A-4335-9511-EB49E7B3228F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,4 +1355,624 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090078DB-29C2-4550-8C8A-4F701FBCE230}">
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="11"/>
+      <c r="D47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="6"/>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="8"/>
+      <c r="D50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="21"/>
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FEAT: updated existing visibility test scripts
see main script changelog and cleaning status spreadsheet for details
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABC2E22-B6A4-499A-B5D8-721EB4E511FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F016C50B-E6F1-4467-B922-60D27E1E601E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>Plotting moved to fcn?</t>
+  </si>
+  <si>
+    <t>Uses FindVertexSkeleton rather than Vskel</t>
   </si>
 </sst>
 </file>
@@ -742,9 +745,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0B7FE0-246A-4335-9511-EB49E7B3228F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H53"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1239,7 @@
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="18"/>
-      <c r="E39" s="17"/>
+      <c r="E39" s="9"/>
       <c r="F39" s="18"/>
       <c r="G39" s="19"/>
       <c r="H39" s="2"/>
@@ -1275,7 +1278,7 @@
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
-      <c r="D42" s="18"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -1316,7 +1319,7 @@
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="18"/>
-      <c r="E45" s="10"/>
+      <c r="E45" s="9"/>
       <c r="F45" s="18"/>
       <c r="G45" s="10"/>
       <c r="H45" s="2"/>
@@ -1363,7 +1366,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1432,7 @@
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -1441,7 +1444,7 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
@@ -1453,7 +1456,7 @@
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
@@ -1467,7 +1470,7 @@
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="25"/>
       <c r="D7" s="18"/>
       <c r="E7" s="25"/>
@@ -1481,7 +1484,7 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="25"/>
       <c r="D8" s="18"/>
       <c r="E8" s="25"/>
@@ -1879,13 +1882,13 @@
         <v>36</v>
       </c>
       <c r="B41" s="9"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="18"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="18"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1894,7 +1897,7 @@
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="28"/>
-      <c r="D42" s="10"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -1907,11 +1910,11 @@
         <v>38</v>
       </c>
       <c r="B43" s="9"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="18"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
       <c r="H43" s="2" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
FEAT: writing separate test script for fcn_Visibility_addObstacle
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F016C50B-E6F1-4467-B922-60D27E1E601E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F1CE0B-9052-454C-91FD-A7C320765B31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -746,8 +746,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
-      <c r="D41" s="18"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
-      <c r="D43" s="18"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -1365,8 +1365,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,12 +1867,12 @@
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="24"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="2" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
FEAT: continuing updates to visibility fcns
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F1CE0B-9052-454C-91FD-A7C320765B31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B89DBF8-D830-4900-B243-A9C754C79796}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -426,9 +426,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,8 +746,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,9 +1238,9 @@
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="18"/>
+      <c r="D39" s="10"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="18"/>
+      <c r="F39" s="10"/>
       <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
@@ -1250,9 +1250,9 @@
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
-      <c r="D40" s="24"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="18"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="2" t="s">
         <v>57</v>
@@ -1304,9 +1304,9 @@
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="D44" s="18"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="18"/>
+      <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="2" t="s">
         <v>58</v>
@@ -1365,8 +1365,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,24 +1843,24 @@
       <c r="A38" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
       <c r="E38" s="23"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1871,8 +1871,8 @@
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="24"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
       <c r="H40" s="2" t="s">
         <v>57</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="9"/>
-      <c r="C42" s="28"/>
+      <c r="C42" s="26"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
@@ -1923,12 +1923,12 @@
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
       <c r="H44" s="2" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
FEAT: 3d visibility plotting moved into fcns
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B89DBF8-D830-4900-B243-A9C754C79796}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12626B98-71C8-4A78-85C0-05BE8BF23C0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Uses FindVertexSkeleton rather than Vskel</t>
+  </si>
+  <si>
+    <t>No other scripts actually appear to be using this</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,8 +430,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,8 +747,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1231,9 @@
       <c r="E38" s="22"/>
       <c r="F38" s="23"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="13"/>
+      <c r="H38" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -1238,9 +1241,9 @@
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="10"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
@@ -1365,8 +1368,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,24 +1846,26 @@
       <c r="A38" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="23"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="13"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FEAT: continued updates to BoundedAStar fcns
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12626B98-71C8-4A78-85C0-05BE8BF23C0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0F0D9C-D57B-4764-9729-8E50BA37C51F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -747,14 +747,14 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
@@ -1168,36 +1168,36 @@
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1227,9 +1227,9 @@
       </c>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
-      <c r="D38" s="23"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="22"/>
-      <c r="F38" s="23"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="13" t="s">
         <v>63</v>
@@ -1321,10 +1321,10 @@
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
-      <c r="D45" s="18"/>
+      <c r="D45" s="9"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="10"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
       <c r="H45" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1368,18 +1368,19 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="7" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
     <col min="8" max="8" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1789,36 +1790,36 @@
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1942,12 +1943,12 @@
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
       <c r="E45" s="18"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
       <c r="H45" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FEAT: continued cleaning of BoundedAStar fcns
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0F0D9C-D57B-4764-9729-8E50BA37C51F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648384ED-2092-48EE-8CDF-B2056C60068C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>No other scripts actually appear to be using this</t>
+  </si>
+  <si>
+    <t>Couldn't really think of what to add as debug plotting for this one</t>
   </si>
 </sst>
 </file>
@@ -747,8 +750,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,13 +979,15 @@
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="2"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1000,12 +1005,12 @@
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1368,8 +1373,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1555,7 @@
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -1586,7 +1591,7 @@
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -1598,19 +1603,21 @@
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="2"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="12"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
@@ -1622,12 +1629,12 @@
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1658,7 +1665,7 @@
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1694,7 +1701,7 @@
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>

</xml_diff>

<commit_message>
FEAT: updates to findEdgeWeights and greedyPlanner
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648384ED-2092-48EE-8CDF-B2056C60068C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1818990-2F82-41D6-A1B2-7D13D78E94B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Couldn't really think of what to add as debug plotting for this one</t>
+  </si>
+  <si>
+    <t>Debug plotting broken but fcn working</t>
   </si>
 </sst>
 </file>
@@ -749,9 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0B7FE0-246A-4335-9511-EB49E7B3228F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,12 +970,12 @@
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1010,8 +1013,10 @@
       <c r="D19" s="10"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="2"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1372,9 +1377,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090078DB-29C2-4550-8C8A-4F701FBCE230}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,11 +1597,11 @@
         <v>13</v>
       </c>
       <c r="B16" s="9"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1630,12 +1635,14 @@
         <v>16</v>
       </c>
       <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="2"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">

</xml_diff>

<commit_message>
FEAT: updates to old BoundedAStar fcns
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1818990-2F82-41D6-A1B2-7D13D78E94B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03235D2-A247-44C0-B56D-43F6448D5961}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -753,8 +753,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,13 +934,15 @@
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="2"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1046,12 +1048,12 @@
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1378,8 +1380,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,11 +1563,11 @@
         <v>10</v>
       </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,11 +1675,11 @@
         <v>19</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1997,5 +1999,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FEAT: updates to createPhantomGoal
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03235D2-A247-44C0-B56D-43F6448D5961}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2BD6FE-695C-45A9-8BC8-A42D0CB39FF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -752,9 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0B7FE0-246A-4335-9511-EB49E7B3228F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,12 +960,12 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="12"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
@@ -1084,7 +1084,7 @@
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -1379,9 +1379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090078DB-29C2-4550-8C8A-4F701FBCE230}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,12 +1586,12 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FEAT: updates to BoundedAStar fcns
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B18036F-F97A-4755-A869-62C7423A9D1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9265E8-44CD-4EBB-B3A6-6008B8C306AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -752,9 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0B7FE0-246A-4335-9511-EB49E7B3228F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,24 +1024,24 @@
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1379,9 +1379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090078DB-29C2-4550-8C8A-4F701FBCE230}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,24 +1650,24 @@
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FEAT: continued updates to old fcns
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mocki\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9265E8-44CD-4EBB-B3A6-6008B8C306AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B74631D-C6F5-4FA8-A0A7-20255CF6E5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
   <si>
     <t>animateTimespacePathPlan</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Debug plotting broken but fcn working</t>
+  </si>
+  <si>
+    <t>Test cases needed demonstrating functionality of all maps</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +315,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -436,6 +445,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,9 +464,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -494,7 +504,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -600,7 +610,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -742,7 +752,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -753,22 +763,22 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="8" max="8" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>43</v>
@@ -792,7 +802,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>42</v>
       </c>
@@ -804,7 +814,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -816,7 +826,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -828,7 +838,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -840,7 +850,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -854,7 +864,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -868,7 +878,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -882,7 +892,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -894,7 +904,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -906,7 +916,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -918,7 +928,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -930,7 +940,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -944,19 +954,19 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -968,7 +978,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -980,7 +990,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -994,7 +1004,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1006,7 +1016,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1032,7 +1042,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1044,7 +1054,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1056,31 +1066,31 @@
       <c r="G22" s="9"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1092,7 +1102,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1104,7 +1114,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1116,7 +1126,7 @@
       <c r="G27" s="12"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -1128,7 +1138,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1140,7 +1150,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1152,7 +1162,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1164,19 +1174,19 @@
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1188,7 +1198,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1200,7 +1210,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1212,7 +1222,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1221,7 +1231,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
         <v>41</v>
       </c>
@@ -1233,7 +1243,7 @@
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>33</v>
       </c>
@@ -1247,7 +1257,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -1259,7 +1269,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -1273,7 +1283,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -1287,7 +1297,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -1299,7 +1309,7 @@
       <c r="G42" s="9"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
@@ -1313,7 +1323,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
@@ -1339,31 +1349,31 @@
       <c r="G45" s="9"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B47" s="11"/>
       <c r="C47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48" s="6"/>
       <c r="C48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="8"/>
       <c r="C50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="21"/>
       <c r="C51" t="s">
         <v>56</v>
@@ -1380,23 +1390,23 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="47.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>55</v>
@@ -1420,7 +1430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>42</v>
       </c>
@@ -1432,7 +1442,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1454,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1456,7 +1466,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1468,7 +1478,7 @@
       <c r="G5" s="25"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1482,7 +1492,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1496,7 +1506,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1510,7 +1520,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1522,7 +1532,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1534,7 +1544,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1546,7 +1556,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1558,7 +1568,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1570,7 +1580,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1582,7 +1592,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1594,7 +1604,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1606,7 +1616,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1620,7 +1630,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1632,7 +1642,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1646,7 +1656,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1658,7 +1668,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1670,7 +1680,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1682,31 +1692,33 @@
       <c r="G22" s="9"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1718,7 +1730,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1730,7 +1742,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1742,7 +1754,7 @@
       <c r="G27" s="12"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -1754,7 +1766,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1766,7 +1778,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1778,7 +1790,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1790,19 +1802,19 @@
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1814,7 +1826,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1826,7 +1838,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1838,7 +1850,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1847,7 +1859,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
         <v>41</v>
       </c>
@@ -1859,7 +1871,7 @@
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>33</v>
       </c>
@@ -1873,7 +1885,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -1885,7 +1897,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -1899,7 +1911,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -1913,7 +1925,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -1927,7 +1939,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
@@ -1941,7 +1953,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
@@ -1955,7 +1967,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
@@ -1967,31 +1979,31 @@
       <c r="G45" s="9"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C47" s="11"/>
       <c r="D47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C48" s="6"/>
       <c r="D48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="7"/>
       <c r="D49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="8"/>
       <c r="D50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="21"/>
       <c r="D51" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
FEAT: updates to AStar test scripts
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mocki\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDF0B31-4D8D-490F-AC4C-CF942A99BDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0464FB24-A9A9-47CF-8A3A-B3C4F35DAC85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -446,6 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,9 +465,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -504,7 +505,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -610,7 +611,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -752,7 +753,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -762,23 +763,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0B7FE0-246A-4335-9511-EB49E7B3228F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="4" width="27.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>43</v>
@@ -802,7 +803,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>42</v>
       </c>
@@ -814,7 +815,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -826,7 +827,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -838,7 +839,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -846,11 +847,11 @@
       <c r="C5" s="9"/>
       <c r="D5" s="17"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="9"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -864,7 +865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -878,7 +879,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -892,7 +893,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -904,7 +905,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -916,7 +917,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -928,7 +929,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -940,7 +941,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -954,7 +955,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -966,7 +967,7 @@
       <c r="G14" s="27"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -978,7 +979,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -990,7 +991,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1016,13 +1017,13 @@
       <c r="G18" s="12"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1030,7 +1031,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1042,7 +1043,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1054,7 +1055,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1066,7 +1067,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1078,7 +1079,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1090,7 +1091,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1102,7 +1103,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1114,7 +1115,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1126,7 +1127,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -1138,7 +1139,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1151,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1162,7 +1163,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1174,7 +1175,7 @@
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1186,7 +1187,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1198,7 +1199,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1210,7 +1211,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1222,7 +1223,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1231,7 +1232,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>41</v>
       </c>
@@ -1243,7 +1244,7 @@
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>33</v>
       </c>
@@ -1257,7 +1258,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -1269,7 +1270,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -1309,7 +1310,7 @@
       <c r="G42" s="9"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
@@ -1349,31 +1350,31 @@
       <c r="G45" s="9"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
       <c r="C47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="21"/>
       <c r="C51" t="s">
         <v>56</v>
@@ -1389,24 +1390,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090078DB-29C2-4550-8C8A-4F701FBCE230}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="47.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>55</v>
@@ -1430,7 +1431,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>42</v>
       </c>
@@ -1442,7 +1443,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1454,59 +1455,59 @@
       <c r="G3" s="14"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1520,7 +1521,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1532,7 +1533,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1544,7 +1545,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1556,7 +1557,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1569,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1580,7 +1581,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1592,7 +1593,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1604,7 +1605,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1616,7 +1617,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1642,7 +1643,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1650,13 +1651,13 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1668,7 +1669,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1680,7 +1681,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1692,7 +1693,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1718,7 +1719,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1730,7 +1731,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1742,7 +1743,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1754,7 +1755,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -1766,7 +1767,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1778,7 +1779,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1790,7 +1791,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1802,7 +1803,7 @@
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1814,7 +1815,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1826,7 +1827,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1838,7 +1839,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1850,7 +1851,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1859,7 +1860,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>41</v>
       </c>
@@ -1871,7 +1872,7 @@
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>33</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -1897,7 +1898,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
@@ -1979,31 +1980,31 @@
       <c r="G45" s="9"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="11"/>
       <c r="D47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="6"/>
       <c r="D48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="8"/>
       <c r="D50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="21"/>
       <c r="D51" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
FEAT: updated bounding polytope BB fcn
</commit_message>
<xml_diff>
--- a/BoundedAStar_CleaningStatus.xlsx
+++ b/BoundedAStar_CleaningStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kxh1031\Documents\GitHub\PathPlanning_GridFreePathPlanners_BoundedAStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68B5A26-3D0E-4D7D-A37D-6738A43143F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4C1B9-EE92-4084-BAB1-D85780765BF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1" xr2:uid="{F0BFAE3D-301B-4181-A03B-E493C29995D8}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>AstarBoundedSetupForTiledPolytopes</t>
   </si>
   <si>
-    <t>calculateBoundingEllipsePolytopeBoundingBox</t>
-  </si>
-  <si>
     <t>calculateBoundingEllipseMinPerimPath</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>Not currently working, missing 3d capabilities for some operations</t>
+  </si>
+  <si>
+    <t>calculateBoundingEllipsePolytope</t>
   </si>
 </sst>
 </file>
@@ -760,8 +760,8 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,30 +778,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -822,7 +822,7 @@
       <c r="F3" s="21"/>
       <c r="G3" s="22"/>
       <c r="H3" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="9"/>
       <c r="H6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -874,12 +874,12 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -888,24 +888,24 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -917,7 +917,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -929,7 +929,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -941,7 +941,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -950,12 +950,12 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -964,12 +964,12 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -981,7 +981,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -993,7 +993,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1002,12 +1002,12 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1028,12 +1028,12 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -1255,12 +1255,12 @@
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
       <c r="H38" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1281,12 +1281,12 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1295,12 +1295,12 @@
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -1321,12 +1321,12 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -1335,12 +1335,12 @@
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -1353,31 +1353,31 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
       <c r="C47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="20"/>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1392,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,30 +1410,30 @@
     <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -1454,7 +1454,7 @@
       <c r="F3" s="26"/>
       <c r="G3" s="22"/>
       <c r="H3" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,12 +1506,12 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="24"/>
@@ -1520,24 +1520,24 @@
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
       <c r="H8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="18"/>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1594,12 +1594,12 @@
       <c r="F14" s="17"/>
       <c r="G14" s="9"/>
       <c r="H14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1632,12 +1632,12 @@
       <c r="F17" s="17"/>
       <c r="G17" s="9"/>
       <c r="H17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="12"/>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1658,12 +1658,12 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1708,12 +1708,12 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="12"/>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -1887,12 +1887,12 @@
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
       <c r="H38" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1913,12 +1913,12 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1927,12 +1927,12 @@
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="25"/>
@@ -1941,12 +1941,12 @@
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -1955,12 +1955,12 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -1969,12 +1969,12 @@
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -1987,31 +1987,31 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="11"/>
       <c r="D47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="6"/>
       <c r="D48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="8"/>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="20"/>
       <c r="D51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>